<commit_message>
fix code, finish tests
</commit_message>
<xml_diff>
--- a/Projects/MARSUAE_SAND/Tests/Data/external_targets.xlsx
+++ b/Projects/MARSUAE_SAND/Tests/Data/external_targets.xlsx
@@ -223,7 +223,7 @@
     <t xml:space="preserve">{"Target": "", "Weight": 15, "kpi_child": "", "KPI Family": "Availability", "kpi_parent": "", "score_logic": "Tiered", "Template Name": "Main Shelf Gum and Confectionary", "KPI Level 2 Name": "Gum &amp; Fruity", "score_cond_score_1": 0, "score_cond_score_2": 0.8, "score_cond_score_3": 1, "score_cond_score_4": "", "score_cond_target_1": 0.89, "score_cond_target_2": 0.96, "score_cond_target_3": 1.01, "score_cond_target_4": "", "exclude_param_type_1": "", "exclude_param_value_1": "", "param_type_2/denom_type": "", "param_value_2/denom_value": "", "param_type_1/numerator_type": "assortment_type", "param_value_1/numerator_value": "NBL - Gum Main"}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"Target": 2, "Weight": 10, "kpi_child": "", "KPI Family": "Block", "kpi_parent": "", "score_logic": "Binary", "Template Name": "Main Shelf Gum and Confectionary", "KPI Level 2 Name": "Gum &amp; Fruity", "score_cond_score_1": "", "score_cond_score_2": "", "score_cond_score_3": "", "score_cond_score_4": "", "score_cond_target_1": "", "score_cond_target_2": "", "score_cond_target_3": "", "score_cond_target_4": "", "exclude_param_type_1": "", "exclude_param_value_1": "", "param_type_2/denom_type": "", "param_value_2/denom_value": "", "param_type_1/numerator_type": "", "param_value_1/numerator_value": ""}</t>
+    <t xml:space="preserve">{"Target": 0.3, "Weight": 10, "kpi_child": "", "KPI Family": "Block", "kpi_parent": "", "score_logic": "Binary", "Template Name": "Main Shelf Gum and Confectionary", "KPI Level 2 Name": "Gum &amp; Fruity", "score_cond_score_1": "", "score_cond_score_2": "", "score_cond_score_3": "", "score_cond_score_4": "", "score_cond_target_1": "", "score_cond_target_2": "", "score_cond_target_3": "", "score_cond_target_4": "", "exclude_param_type_1": "", "exclude_param_value_1": "", "param_type_2/denom_type": "", "param_value_2/denom_value": "", "param_type_1/numerator_type": "", "param_value_1/numerator_value": ""}</t>
   </si>
   <si>
     <t xml:space="preserve">{"Target": 1, "Weight": 40, "kpi_child": ["SOS - Gum/Fruity Checkout", "POI Compliance - Gum / Fruity Checkout"], "KPI Family": "Kpi Combination", "kpi_parent": "", "score_logic": "Binary", "Template Name": "Checkout Gum &amp; Confectionary", "KPI Level 2 Name": "Gum &amp; Fruity", "score_cond_score_1": "", "score_cond_score_2": "", "score_cond_score_3": "", "score_cond_score_4": "", "score_cond_target_1": "", "score_cond_target_2": "", "score_cond_target_3": "", "score_cond_target_4": "", "exclude_param_type_1": "", "exclude_param_value_1": "", "param_type_2/denom_type": "", "param_value_2/denom_value": "", "param_type_1/numerator_type": "", "param_value_1/numerator_value": ""}</t>
@@ -388,13 +388,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,7 +443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -472,7 +472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -501,7 +501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -530,7 +530,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>46</v>
       </c>
@@ -559,7 +559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>47</v>
       </c>
@@ -588,7 +588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>48</v>
       </c>
@@ -617,7 +617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>49</v>
       </c>
@@ -675,7 +675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>51</v>
       </c>
@@ -704,7 +704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>52</v>
       </c>
@@ -733,7 +733,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>53</v>
       </c>
@@ -762,7 +762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>54</v>
       </c>
@@ -791,7 +791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>55</v>
       </c>
@@ -820,7 +820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>56</v>
       </c>
@@ -849,7 +849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>57</v>
       </c>
@@ -878,7 +878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>58</v>
       </c>
@@ -936,7 +936,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>60</v>
       </c>
@@ -965,7 +965,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>61</v>
       </c>
@@ -994,7 +994,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>62</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>63</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>64</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>65</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>66</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>67</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>68</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>69</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>70</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>71</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>72</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>73</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>74</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>75</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>76</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>77</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>78</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>79</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>80</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>81</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>82</v>
       </c>
@@ -1604,13 +1604,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J41">
-    <filterColumn colId="9">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Checkout Penetration - Chocolate"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
add gum sos additional condition
</commit_message>
<xml_diff>
--- a/Projects/MARSUAE_SAND/Tests/Data/external_targets.xlsx
+++ b/Projects/MARSUAE_SAND/Tests/Data/external_targets.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
   <si>
     <t xml:space="preserve">pk</t>
   </si>
@@ -266,6 +267,15 @@
   </si>
   <si>
     <t xml:space="preserve">{"Target": 0.55, "Weight": 50, "kpi_child": "", "KPI Family": "Linear SOS", "kpi_parent": "", "score_logic": "Relative Score", "Template Name": "Main Shelf Pet food", "KPI Level 2 Name": "Pet Food", "score_cond_score_1": "", "score_cond_score_2": "", "score_cond_score_3": "", "score_cond_score_4": "", "score_cond_target_1": "", "score_cond_target_2": "", "score_cond_target_3": "", "score_cond_target_4": "", "exclude_param_type_1": "", "exclude_param_value_1": "", "param_type_2/denom_type": "category_fk", "param_value_2/denom_value": 5, "param_type_1/numerator_type": "manufacturer_fk", "param_value_1/numerator_value": 2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"store_att_name_1": "store_type", "store_att_value_1": "Supers A"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Target": "", "Weight": 20, "kpi_child": "", "KPI Family": "Linear SOS", "kpi_parent": "", "score_logic": "Tiered", "Template Name": "Checkout Gum &amp; Confectionary", "KPI Level 2 Name": "Gum &amp; Fruity", "score_cond_score_1": 0, "score_cond_score_2": 0.75, "score_cond_score_3": 1, "score_cond_score_4": "", "score_cond_target_1": 0.6, "score_cond_target_2": 0.7, "score_cond_target_3": 1.01, "score_cond_target_4": "", "exclude_param_type_1": "sub_category_fk", "exclude_param_type_2": "product_type", "exclude_param_value_1": 20, "exclude_param_value_2": ["Other", "Empty"], "param_type_2/denom_type": "category_fk", "param_value_2/denom_value": 10, "param_type_1/numerator_type": "manufacturer_fk", "param_value_1/numerator_value": 762, "exclude_param_2_exception_type": "brand_fk", "exclude_param_2_exception_value": 82}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Target": "", "Weight": 15, "kpi_child": "", "KPI Family": "Linear SOS", "kpi_parent": "", "score_logic": "Tiered", "Template Name": "Main Shelf Gum and Confectionary", "KPI Level 2 Name": "Gum &amp; Fruity", "score_cond_score_1": 0, "score_cond_score_2": 0.8, "score_cond_score_3": 0.9, "score_cond_score_4": 1, "score_cond_target_1": 0.58, "score_cond_target_2": 0.6, "score_cond_target_3": 0.62, "score_cond_target_4": 1.01, "exclude_param_type_1": "sub_category_fk", "exclude_param_type_2": "product_type", "exclude_param_value_1": 20, "exclude_param_value_2": ["Other", "Empty"], "param_type_2/denom_type": "category_fk", "param_value_2/denom_value": 10, "param_type_1/numerator_type": "manufacturer_fk", "param_value_1/numerator_value": 762, "exclude_param_2_exception_type": "brand_fk", "exclude_param_2_exception_value": 82}</t>
   </si>
 </sst>
 </file>
@@ -391,23 +401,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="64.5910931174089"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="141.125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9311740890688"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.6801619433198"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="144.801619433198"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1601,6 +1611,122 @@
       </c>
       <c r="J41" s="0" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>3031</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>43468</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>43677.5600115741</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>3032</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>43468</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>43677.5600115741</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>3030</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>43468</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>43677.5600115741</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>3029</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>43468</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>43677.5600115741</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>